<commit_message>
Add and corrected some missing names and titles
</commit_message>
<xml_diff>
--- a/xls/UmaMusume Uma Name Translation List.xlsx
+++ b/xls/UmaMusume Uma Name Translation List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\UmaMusume\Tools\UmaCruiseTranslation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\starg\Documents\GitHub\umacruise-english-patch\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6846223-A9B8-482E-826B-6F6769F8C58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7929DBC6-26DC-43FD-BA9B-88ED021FC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{167422E0-6C86-4113-A42F-2B95032D97C4}"/>
+    <workbookView xWindow="20280" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{167422E0-6C86-4113-A42F-2B95032D97C4}"/>
   </bookViews>
   <sheets>
     <sheet name="uma-name" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'uma-name'!$A$1:$B$78</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'uma-name'!$A$1:$B$79</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>text</t>
   </si>
@@ -500,9 +498,6 @@
     <t>Otonashi Etsuko</t>
   </si>
   <si>
-    <t>桐生院トレーナー</t>
-  </si>
-  <si>
     <t>Kiryuin Aoi</t>
   </si>
   <si>
@@ -513,6 +508,15 @@
   </si>
   <si>
     <t>translation</t>
+  </si>
+  <si>
+    <t>桐生院葵</t>
+  </si>
+  <si>
+    <t>樫本理子</t>
+  </si>
+  <si>
+    <t>Kashimoto Riko</t>
   </si>
 </sst>
 </file>
@@ -587,7 +591,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F13D0B91-540A-442E-B6B9-E217E0CF48C2}" name="uma_name" displayName="uma_name" ref="A1:B78" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F13D0B91-540A-442E-B6B9-E217E0CF48C2}" name="uma_name" displayName="uma_name" ref="A1:B79" tableType="queryTable" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{528C3586-6EF5-429C-B73C-1DD974FFAB9F}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{8AD93808-6557-41C5-A6D8-BF4EDDDF4237}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="0"/>
@@ -597,7 +601,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -893,13 +897,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E186FB1F-3697-4458-87FD-8CC556AC01E9}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
@@ -910,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,18 +1519,26 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>154</v>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>